<commit_message>
added camera code and an updated of the accountability
</commit_message>
<xml_diff>
--- a/Cost/Accountability.xlsx
+++ b/Cost/Accountability.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="26">
   <si>
     <t>Description</t>
   </si>
@@ -76,6 +76,24 @@
   </si>
   <si>
     <t>Total cost</t>
+  </si>
+  <si>
+    <t>Canon Elph 330 S</t>
+  </si>
+  <si>
+    <t>Canon</t>
+  </si>
+  <si>
+    <t>RC 6 channels</t>
+  </si>
+  <si>
+    <t>StockRC</t>
+  </si>
+  <si>
+    <t>Battery charger</t>
+  </si>
+  <si>
+    <t>Servo wire x5</t>
   </si>
 </sst>
 </file>
@@ -433,7 +451,7 @@
   <dimension ref="A1:H36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -623,9 +641,21 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F8" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8">
+        <v>167.13</v>
+      </c>
+      <c r="D8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" s="1">
+        <f t="shared" si="0"/>
+        <v>167.13</v>
       </c>
       <c r="G8" s="1" t="str">
         <f t="shared" si="0"/>
@@ -637,9 +667,21 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F9" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9">
+        <v>71.569999999999993</v>
+      </c>
+      <c r="D9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" s="1">
+        <f t="shared" si="0"/>
+        <v>71.569999999999993</v>
       </c>
       <c r="G9" s="1" t="str">
         <f t="shared" si="0"/>
@@ -651,9 +693,21 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F10" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10">
+        <v>68.62</v>
+      </c>
+      <c r="D10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F10" s="1">
+        <f t="shared" si="0"/>
+        <v>68.62</v>
       </c>
       <c r="G10" s="1" t="str">
         <f t="shared" si="0"/>
@@ -665,9 +719,21 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F11" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="A11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11">
+        <v>14.54</v>
+      </c>
+      <c r="D11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F11" s="1">
+        <f t="shared" si="0"/>
+        <v>14.54</v>
       </c>
       <c r="G11" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1006,7 +1072,7 @@
       </c>
       <c r="F36">
         <f>SUM(F2:F34)</f>
-        <v>322.21999999999997</v>
+        <v>644.07999999999993</v>
       </c>
       <c r="G36">
         <f t="shared" ref="G36:H36" si="1">SUM(G2:G34)</f>

</xml_diff>

<commit_message>
Version with BIG things in mind. More to come for julio from home depot and some other BS
</commit_message>
<xml_diff>
--- a/Cost/Accountability.xlsx
+++ b/Cost/Accountability.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="30" windowWidth="10515" windowHeight="5445"/>
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="53">
   <si>
     <t>Description</t>
   </si>
@@ -154,6 +154,27 @@
   </si>
   <si>
     <t>APM Chino</t>
+  </si>
+  <si>
+    <t>Radio Chino</t>
+  </si>
+  <si>
+    <t>Cama s100 Canon</t>
+  </si>
+  <si>
+    <t>3DR</t>
+  </si>
+  <si>
+    <t>Ardupilot</t>
+  </si>
+  <si>
+    <t>Camara ELPH s130</t>
+  </si>
+  <si>
+    <t>Radio Spektrum</t>
+  </si>
+  <si>
+    <t>Speed Controller</t>
   </si>
 </sst>
 </file>
@@ -510,8 +531,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1169,13 +1190,25 @@
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>44</v>
+      </c>
+      <c r="B26" t="s">
+        <v>46</v>
+      </c>
+      <c r="C26">
+        <v>21.8</v>
+      </c>
+      <c r="D26" t="s">
+        <v>8</v>
+      </c>
       <c r="F26" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="G26" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="G26" s="1">
+        <f t="shared" si="0"/>
+        <v>21.8</v>
       </c>
       <c r="H26" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1183,13 +1216,25 @@
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>17</v>
+      </c>
+      <c r="B27" t="s">
+        <v>47</v>
+      </c>
+      <c r="C27">
+        <v>156.6</v>
+      </c>
+      <c r="D27" t="s">
+        <v>8</v>
+      </c>
       <c r="F27" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="G27" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="G27" s="1">
+        <f t="shared" si="0"/>
+        <v>156.6</v>
       </c>
       <c r="H27" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1197,6 +1242,18 @@
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>48</v>
+      </c>
+      <c r="B28" t="s">
+        <v>49</v>
+      </c>
+      <c r="C28">
+        <v>243</v>
+      </c>
+      <c r="D28" t="s">
+        <v>9</v>
+      </c>
       <c r="F28" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1205,12 +1262,24 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="H28" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="H28" s="1">
+        <f t="shared" si="0"/>
+        <v>243</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>21</v>
+      </c>
+      <c r="B29" t="s">
+        <v>50</v>
+      </c>
+      <c r="C29">
+        <v>100</v>
+      </c>
+      <c r="D29" t="s">
+        <v>9</v>
+      </c>
       <c r="F29" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1219,12 +1288,24 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="H29" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="H29" s="1">
+        <f t="shared" si="0"/>
+        <v>100</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B30" t="s">
+        <v>51</v>
+      </c>
+      <c r="C30">
+        <v>166</v>
+      </c>
+      <c r="D30" t="s">
+        <v>9</v>
+      </c>
       <c r="F30" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1233,12 +1314,24 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="H30" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="H30" s="1">
+        <f t="shared" si="0"/>
+        <v>166</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>28</v>
+      </c>
+      <c r="B31" t="s">
+        <v>52</v>
+      </c>
+      <c r="C31">
+        <v>55</v>
+      </c>
+      <c r="D31" t="s">
+        <v>9</v>
+      </c>
       <c r="F31" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1247,9 +1340,9 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="H31" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="H31" s="1">
+        <f t="shared" si="0"/>
+        <v>55</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -1710,11 +1803,11 @@
       </c>
       <c r="G64">
         <f>SUM(G2:G34)</f>
-        <v>265.5</v>
+        <v>443.9</v>
       </c>
       <c r="H64">
         <f>SUM(H2:H34)</f>
-        <v>0</v>
+        <v>564</v>
       </c>
     </row>
   </sheetData>

</xml_diff>